<commit_message>
Change format of table
</commit_message>
<xml_diff>
--- a/Хронология.xlsx
+++ b/Хронология.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20416"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PC\Downloads\ТСПП\ЛР5\site\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C66FDCF-81AF-4D43-8AB4-581159461D75}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="30" windowWidth="20115" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="30" windowWidth="20115" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -141,8 +147,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -159,37 +165,29 @@
       <charset val="204"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="8">
+  <borders count="2">
     <border>
       <left/>
       <right/>
       <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
       <bottom/>
       <diagonal/>
     </border>
@@ -202,87 +200,112 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+    <cellStyle name="Звичайний" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="3">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{C33EF0EA-AE71-4F45-8519-028EBFAC0A62}" name="Таблиця2" displayName="Таблиця2" ref="A1:F14" totalsRowShown="0" headerRowDxfId="0" tableBorderDxfId="2">
+  <autoFilter ref="A1:F14" xr:uid="{34453843-D3C2-4DDB-BE93-1783DA910E08}"/>
+  <tableColumns count="6">
+    <tableColumn id="1" xr3:uid="{B24B5359-B675-4719-B0F2-D9943EC5FC12}" name="Название" dataDxfId="1"/>
+    <tableColumn id="2" xr3:uid="{F3F27476-B68C-428D-990F-CD67CC1E5AC7}" name="Год"/>
+    <tableColumn id="3" xr3:uid="{73FAED80-616C-4B3C-BABE-988F2332EDF9}" name="Категория"/>
+    <tableColumn id="4" xr3:uid="{0F7E31C8-678F-46DD-BE18-17663E6C7D31}" name="Количество серий"/>
+    <tableColumn id="5" xr3:uid="{4D478B12-641A-4647-B0D0-9873C76B2F53}" name="Продолжительность"/>
+    <tableColumn id="7" xr3:uid="{7441C339-4E77-4DD8-B044-A2112D414A1D}" name="Сюжет"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
   <a:themeElements>
-    <a:clrScheme name="Стандартная">
+    <a:clrScheme name="Офіс">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -320,9 +343,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Стандартная">
+    <a:fontScheme name="Офіс">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -354,9 +377,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -388,9 +429,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Стандартная">
+    <a:fmtScheme name="Офіс">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -563,45 +622,45 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G14"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:F14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="41.85546875" customWidth="1"/>
     <col min="2" max="2" width="20.28515625" customWidth="1"/>
     <col min="3" max="3" width="19.140625" customWidth="1"/>
-    <col min="4" max="4" width="17.85546875" customWidth="1"/>
-    <col min="5" max="5" width="19.5703125" customWidth="1"/>
-    <col min="6" max="6" width="11.7109375" customWidth="1"/>
-    <col min="7" max="7" width="11.85546875" customWidth="1"/>
+    <col min="4" max="4" width="19.5703125" customWidth="1"/>
+    <col min="5" max="5" width="22.140625" customWidth="1"/>
+    <col min="6" max="6" width="11.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" customHeight="1">
-      <c r="A1" s="8" t="s">
+    <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="13" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="10"/>
-      <c r="G1" s="11" t="s">
+      <c r="F1" s="4" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="15.75" customHeight="1">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -616,11 +675,10 @@
       <c r="E2" t="s">
         <v>32</v>
       </c>
-      <c r="F2" s="1"/>
-      <c r="G2" s="12"/>
-    </row>
-    <row r="3" spans="1:7">
-      <c r="A3" s="2" t="s">
+      <c r="F2" s="6"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B3" s="1" t="s">
@@ -636,10 +694,9 @@
         <v>33</v>
       </c>
       <c r="F3" s="1"/>
-      <c r="G3" s="3"/>
-    </row>
-    <row r="4" spans="1:7">
-      <c r="A4" s="2" t="s">
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B4" s="1" t="s">
@@ -655,10 +712,9 @@
         <v>34</v>
       </c>
       <c r="F4" s="1"/>
-      <c r="G4" s="3"/>
-    </row>
-    <row r="5" spans="1:7">
-      <c r="A5" s="2" t="s">
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B5" s="1" t="s">
@@ -674,10 +730,9 @@
         <v>33</v>
       </c>
       <c r="F5" s="1"/>
-      <c r="G5" s="3"/>
-    </row>
-    <row r="6" spans="1:7">
-      <c r="A6" s="4" t="s">
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
         <v>20</v>
       </c>
       <c r="B6" s="1" t="s">
@@ -693,10 +748,9 @@
         <v>35</v>
       </c>
       <c r="F6" s="1"/>
-      <c r="G6" s="3"/>
-    </row>
-    <row r="7" spans="1:7">
-      <c r="A7" s="4" t="s">
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
         <v>23</v>
       </c>
       <c r="B7" s="1" t="s">
@@ -712,10 +766,9 @@
         <v>35</v>
       </c>
       <c r="F7" s="1"/>
-      <c r="G7" s="3"/>
-    </row>
-    <row r="8" spans="1:7">
-      <c r="A8" s="2" t="s">
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B8" s="1" t="s">
@@ -731,10 +784,9 @@
         <v>36</v>
       </c>
       <c r="F8" s="1"/>
-      <c r="G8" s="3"/>
-    </row>
-    <row r="9" spans="1:7">
-      <c r="A9" s="4" t="s">
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
         <v>17</v>
       </c>
       <c r="B9" s="1" t="s">
@@ -750,10 +802,9 @@
         <v>37</v>
       </c>
       <c r="F9" s="1"/>
-      <c r="G9" s="3"/>
-    </row>
-    <row r="10" spans="1:7">
-      <c r="A10" s="4" t="s">
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="5" t="s">
         <v>25</v>
       </c>
       <c r="B10" s="1" t="s">
@@ -769,10 +820,9 @@
         <v>35</v>
       </c>
       <c r="F10" s="1"/>
-      <c r="G10" s="3"/>
-    </row>
-    <row r="11" spans="1:7">
-      <c r="A11" s="2"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="1"/>
       <c r="B11" s="1" t="s">
         <v>27</v>
       </c>
@@ -786,10 +836,9 @@
         <v>35</v>
       </c>
       <c r="F11" s="1"/>
-      <c r="G11" s="3"/>
-    </row>
-    <row r="12" spans="1:7">
-      <c r="A12" s="2"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="1"/>
       <c r="B12" s="1" t="s">
         <v>28</v>
       </c>
@@ -803,71 +852,71 @@
         <v>35</v>
       </c>
       <c r="F12" s="1"/>
-      <c r="G12" s="3"/>
-    </row>
-    <row r="13" spans="1:7">
-      <c r="A13" s="4" t="s">
-        <v>19</v>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="5" t="s">
+        <v>10</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C13" t="s">
-        <v>30</v>
+        <v>11</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>29</v>
       </c>
       <c r="D13" s="1">
         <v>1</v>
       </c>
-      <c r="E13" t="s">
+      <c r="E13" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="F13" s="1"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C14" t="s">
+        <v>30</v>
+      </c>
+      <c r="D14" s="1">
+        <v>1</v>
+      </c>
+      <c r="E14" t="s">
         <v>38</v>
       </c>
-      <c r="F13" s="1"/>
-      <c r="G13" s="3"/>
-    </row>
-    <row r="14" spans="1:7">
-      <c r="A14" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B14" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="D14" s="5">
-        <v>1</v>
-      </c>
-      <c r="E14" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="F14" s="5"/>
-      <c r="G14" s="6"/>
+      <c r="F14" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>